<commit_message>
added animations for horizontal bow attacks and implemented ground and jump bow animations
</commit_message>
<xml_diff>
--- a/animationList.xlsx
+++ b/animationList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\Desktop\Projects\game_9_30_20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendan\Desktop\Projects\game_9_30_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB379FA-D5B7-4842-A09F-DD353A1804C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF73345-AF2D-49C8-97E5-CA61FE3BE2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14304" yWindow="3504" windowWidth="17280" windowHeight="8964" xr2:uid="{9FFFA082-AA26-4DED-8532-562E7B011087}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FFFA082-AA26-4DED-8532-562E7B011087}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="71">
   <si>
     <t>no weapon</t>
   </si>
@@ -131,24 +131,6 @@
     <t>wallSwing</t>
   </si>
   <si>
-    <t>idleBow</t>
-  </si>
-  <si>
-    <t>runBow</t>
-  </si>
-  <si>
-    <t>jumpBow</t>
-  </si>
-  <si>
-    <t>wallSlideBow</t>
-  </si>
-  <si>
-    <t>ledgeGrabBow</t>
-  </si>
-  <si>
-    <t>fallBow</t>
-  </si>
-  <si>
     <t>complete?</t>
   </si>
   <si>
@@ -182,36 +164,6 @@
     <t>ledgeSwordSheath</t>
   </si>
   <si>
-    <t>wallBowDraw</t>
-  </si>
-  <si>
-    <t>ledgeBowDraw</t>
-  </si>
-  <si>
-    <t>wallBowSheath</t>
-  </si>
-  <si>
-    <t>ledgeBowSheath</t>
-  </si>
-  <si>
-    <t>groundNotch</t>
-  </si>
-  <si>
-    <t>groundRelease</t>
-  </si>
-  <si>
-    <t>groundHoldLoop</t>
-  </si>
-  <si>
-    <t>airNotch</t>
-  </si>
-  <si>
-    <t>airHoldLoop</t>
-  </si>
-  <si>
-    <t>airRelease</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -242,30 +194,6 @@
     <t>fallSwordSheath</t>
   </si>
   <si>
-    <t>runBowDraw</t>
-  </si>
-  <si>
-    <t>idleBowDraw</t>
-  </si>
-  <si>
-    <t>jumpBowDraw</t>
-  </si>
-  <si>
-    <t>fallBowDraw</t>
-  </si>
-  <si>
-    <t>idleBowSheath</t>
-  </si>
-  <si>
-    <t>runBowSheath</t>
-  </si>
-  <si>
-    <t>jumpBowSheath</t>
-  </si>
-  <si>
-    <t>fallBowSheath</t>
-  </si>
-  <si>
     <t>idleSwing1</t>
   </si>
   <si>
@@ -279,6 +207,45 @@
   </si>
   <si>
     <t>collision box?</t>
+  </si>
+  <si>
+    <t>jumpNotch</t>
+  </si>
+  <si>
+    <t>jumpHoldLoop</t>
+  </si>
+  <si>
+    <t>jumpRelease</t>
+  </si>
+  <si>
+    <t>fallNotch</t>
+  </si>
+  <si>
+    <t>fallRelease</t>
+  </si>
+  <si>
+    <t>fallHoldLoop</t>
+  </si>
+  <si>
+    <t>runNotch</t>
+  </si>
+  <si>
+    <t>runHoldLoop</t>
+  </si>
+  <si>
+    <t>runRelease</t>
+  </si>
+  <si>
+    <t>idleNotch</t>
+  </si>
+  <si>
+    <t>idleHoldLoop</t>
+  </si>
+  <si>
+    <t>idleRelease</t>
+  </si>
+  <si>
+    <t>numFrames</t>
   </si>
 </sst>
 </file>
@@ -322,10 +289,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,627 +610,895 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615B73A-1EEF-42FC-96B9-C7826987D3A1}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="J9" s="3">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
       </c>
       <c r="E13" t="s">
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="J13" s="3">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" t="s">
         <v>59</v>
       </c>
-      <c r="G14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
+      <c r="J16" s="3">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="3">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" t="s">
         <v>62</v>
       </c>
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G25" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
-      </c>
-      <c r="I29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>59</v>
-      </c>
-      <c r="I30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s">
-        <v>59</v>
-      </c>
-      <c r="I31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="H36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G37" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="H37" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented slightly buggy magic projectiles
</commit_message>
<xml_diff>
--- a/animationList.xlsx
+++ b/animationList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendan\Desktop\Projects\game_9_30_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601DFAC-E85A-485B-9BED-D00FDB3DA303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432B47AC-4500-4E89-BFCA-D017142513F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FFFA082-AA26-4DED-8532-562E7B011087}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="70">
   <si>
     <t>no weapon</t>
   </si>
@@ -610,7 +610,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,6 +743,9 @@
       <c r="Q2" t="s">
         <v>33</v>
       </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -794,6 +797,9 @@
         <v>33</v>
       </c>
       <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -849,6 +855,9 @@
       <c r="Q4" t="s">
         <v>33</v>
       </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -902,6 +911,9 @@
       <c r="Q5" t="s">
         <v>33</v>
       </c>
+      <c r="R5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -955,6 +967,9 @@
       <c r="Q6" t="s">
         <v>33</v>
       </c>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1008,6 +1023,9 @@
       <c r="Q7" t="s">
         <v>33</v>
       </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J8" s="3"/>
@@ -1065,6 +1083,9 @@
       <c r="Q9" t="s">
         <v>33</v>
       </c>
+      <c r="R9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1118,6 +1139,9 @@
       <c r="Q10" t="s">
         <v>33</v>
       </c>
+      <c r="R10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1330,6 +1354,9 @@
       <c r="Q14" t="s">
         <v>33</v>
       </c>
+      <c r="R14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
@@ -1369,6 +1396,9 @@
         <v>33</v>
       </c>
       <c r="Q15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed character atlas to not have cast loops and removed all sword draws and sheaths
</commit_message>
<xml_diff>
--- a/animationList.xlsx
+++ b/animationList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendan\Desktop\Projects\game_9_30_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432B47AC-4500-4E89-BFCA-D017142513F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C567BC-BC35-4D89-A42B-FD526CF18794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FFFA082-AA26-4DED-8532-562E7B011087}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="65">
   <si>
     <t>no weapon</t>
   </si>
@@ -210,21 +210,6 @@
   </si>
   <si>
     <t>fallCast</t>
-  </si>
-  <si>
-    <t>idleCastLoop</t>
-  </si>
-  <si>
-    <t>runCastLoop</t>
-  </si>
-  <si>
-    <t>jumpCastLoop</t>
-  </si>
-  <si>
-    <t>fallCastLoop</t>
-  </si>
-  <si>
-    <t>wallSlideCastLoop</t>
   </si>
   <si>
     <t>idleGlove</t>
@@ -610,7 +595,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +717,7 @@
         <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O2" s="3">
         <v>4</v>
@@ -741,9 +726,6 @@
         <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -788,7 +770,7 @@
         <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O3" s="3">
         <v>7</v>
@@ -797,9 +779,6 @@
         <v>33</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -844,7 +823,7 @@
         <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O4" s="3">
         <v>2</v>
@@ -853,9 +832,6 @@
         <v>33</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -900,7 +876,7 @@
         <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="O5" s="3">
         <v>2</v>
@@ -909,9 +885,6 @@
         <v>33</v>
       </c>
       <c r="Q5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -956,7 +929,7 @@
         <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O6" s="3">
         <v>4</v>
@@ -965,9 +938,6 @@
         <v>33</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1012,7 +982,7 @@
         <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O7" s="3">
         <v>2</v>
@@ -1021,9 +991,6 @@
         <v>33</v>
       </c>
       <c r="Q7" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1075,15 +1042,12 @@
         <v>54</v>
       </c>
       <c r="O9" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P9" t="s">
         <v>33</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1131,15 +1095,12 @@
         <v>55</v>
       </c>
       <c r="O10" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P10" t="s">
         <v>33</v>
       </c>
       <c r="Q10" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1187,7 +1148,7 @@
         <v>56</v>
       </c>
       <c r="O11" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P11" t="s">
         <v>33</v>
@@ -1240,7 +1201,7 @@
         <v>58</v>
       </c>
       <c r="O12" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P12" t="s">
         <v>33</v>
@@ -1293,7 +1254,7 @@
         <v>57</v>
       </c>
       <c r="O13" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P13" t="s">
         <v>33</v>
@@ -1342,21 +1303,7 @@
       <c r="M14" t="s">
         <v>33</v>
       </c>
-      <c r="N14" t="s">
-        <v>59</v>
-      </c>
-      <c r="O14" s="3">
-        <v>4</v>
-      </c>
-      <c r="P14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R14" t="s">
-        <v>33</v>
-      </c>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
@@ -1386,21 +1333,7 @@
       <c r="M15" t="s">
         <v>33</v>
       </c>
-      <c r="N15" t="s">
-        <v>60</v>
-      </c>
-      <c r="O15" s="3">
-        <v>4</v>
-      </c>
-      <c r="P15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>33</v>
-      </c>
-      <c r="R15" t="s">
-        <v>33</v>
-      </c>
+      <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
@@ -1430,20 +1363,9 @@
       <c r="M16" t="s">
         <v>33</v>
       </c>
-      <c r="N16" t="s">
-        <v>61</v>
-      </c>
-      <c r="O16" s="3">
-        <v>4</v>
-      </c>
-      <c r="P16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>25</v>
       </c>
@@ -1471,20 +1393,9 @@
       <c r="M17" t="s">
         <v>33</v>
       </c>
-      <c r="N17" t="s">
-        <v>62</v>
-      </c>
-      <c r="O17" s="3">
-        <v>4</v>
-      </c>
-      <c r="P17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>43</v>
       </c>
@@ -1500,20 +1411,9 @@
       <c r="M18" t="s">
         <v>33</v>
       </c>
-      <c r="N18" t="s">
-        <v>63</v>
-      </c>
-      <c r="O18" s="3">
-        <v>4</v>
-      </c>
-      <c r="P18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>45</v>
       </c>
@@ -1531,7 +1431,7 @@
       </c>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>44</v>
       </c>

</xml_diff>